<commit_message>
Kontrollera indata för saveTask funkar
</commit_message>
<xml_diff>
--- a/tidsapp/Dokumentation/Testprotokoll.xlsx
+++ b/tidsapp/Dokumentation/Testprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Ovningar\tidsapp\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E863F456-276A-419F-9DC8-E3987C60651F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD094E6-C64E-40CB-8E4A-F0279AF01599}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="3720" xr2:uid="{746CABA9-F874-49F1-AADB-2D0BDB8C27DF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="105">
   <si>
     <t>Testprotokoll, Tidsredovisning</t>
   </si>
@@ -183,9 +183,6 @@
     <t>saveActivity.php activity='ny'</t>
   </si>
   <si>
-    <t>OK id=5 Aktiviteten sparades</t>
-  </si>
-  <si>
     <t>saveActivity.php?id=-1 activity='nygammal'</t>
   </si>
   <si>
@@ -213,7 +210,137 @@
     <t>Fel (405) Anropa med POST</t>
   </si>
   <si>
-    <t>Fel (400) activity vara tom</t>
+    <t>OK id=XX Aktiviteten sparades</t>
+  </si>
+  <si>
+    <t>OK id=4 Spara lyckades</t>
+  </si>
+  <si>
+    <t>saveActivity.php?id=5 INGEN activity</t>
+  </si>
+  <si>
+    <t>Fel (400) activity saknas</t>
+  </si>
+  <si>
+    <t>saveActivity.php?id=5 activity=''</t>
+  </si>
+  <si>
+    <t>OK result=true message=1 post uppdaterades</t>
+  </si>
+  <si>
+    <t>saveActivity.php?id=5 activity='gammal'</t>
+  </si>
+  <si>
+    <t>OK result=false message=Inga poster uppdaterades</t>
+  </si>
+  <si>
+    <t>Radera aktivitet</t>
+  </si>
+  <si>
+    <t>deleteActivity.php via GET</t>
+  </si>
+  <si>
+    <t>deleteActivity.php via POST</t>
+  </si>
+  <si>
+    <t>deleteActivity.php id=-1</t>
+  </si>
+  <si>
+    <t>deleteActivity.php id=tre</t>
+  </si>
+  <si>
+    <t>deleteActivity.php id=300</t>
+  </si>
+  <si>
+    <t>OK Inga poster raderades</t>
+  </si>
+  <si>
+    <t>deleteActivity.php id=1</t>
+  </si>
+  <si>
+    <t>Fel (400) Inga poster raderades, id används i Tasks</t>
+  </si>
+  <si>
+    <t>deleteActivity-php id=5</t>
+  </si>
+  <si>
+    <t>OK 1 post raderades</t>
+  </si>
+  <si>
+    <t>deleteActivity.php id=</t>
+  </si>
+  <si>
+    <t>OK result=false message=Inga poster raderades</t>
+  </si>
+  <si>
+    <t>OK result=true message=1 post raderades</t>
+  </si>
+  <si>
+    <t>Fel (400) Fel vid radering,
+Angivet id (1) används</t>
+  </si>
+  <si>
+    <t>Spara uppgift</t>
+  </si>
+  <si>
+    <t>saveTask.php via GET</t>
+  </si>
+  <si>
+    <t>saveTask.php via POST utan parametrar</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar time=-1</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar time=tre</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar time=12:00</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar date=-1</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar date=tre</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar date=2001-02-29</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar activityid=-1</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar activityid=tre</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar activityid=300</t>
+  </si>
+  <si>
+    <t>saveTask.php med alla parametrar description=''</t>
+  </si>
+  <si>
+    <t>Fel (400) activityid saknas, time saknas, date saknas</t>
+  </si>
+  <si>
+    <t>Fel (400) felaktigt angiven time</t>
+  </si>
+  <si>
+    <t>Fel (400) felaktigt angiven date</t>
+  </si>
+  <si>
+    <t>Fel (400) Får inte spara mer än 8 timmar per uppgift</t>
+  </si>
+  <si>
+    <t>Fel (400) felaktig activityid</t>
+  </si>
+  <si>
+    <t>Fel (400) angiven aktivitet saknas</t>
+  </si>
+  <si>
+    <t>OK posten sparades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saveTask.php med alla parametrar </t>
   </si>
 </sst>
 </file>
@@ -294,11 +421,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -312,6 +436,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -630,501 +760,933 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C2BE4A-9F0B-44D4-B350-F96D596D6606}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>46023</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>46023</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>46023</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>46023</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>46023</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>11324</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>11324</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>11324</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>11324</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>11324</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>11324</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>11324</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>11324</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>11324</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>11324</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>11324</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>11324</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="7">
+        <v>44593</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="7">
+        <v>44593</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44593</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7">
+        <v>44593</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="D25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="D30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B32" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>59</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixat sparaTask och lagt till ram för uppdatering
</commit_message>
<xml_diff>
--- a/tidsapp/Dokumentation/Testprotokoll.xlsx
+++ b/tidsapp/Dokumentation/Testprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Ovningar\tidsapp\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD094E6-C64E-40CB-8E4A-F0279AF01599}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585B0CB4-9EED-439F-A265-3804AF3D4AA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="3720" xr2:uid="{746CABA9-F874-49F1-AADB-2D0BDB8C27DF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="121">
   <si>
     <t>Testprotokoll, Tidsredovisning</t>
   </si>
@@ -341,6 +341,54 @@
   </si>
   <si>
     <t xml:space="preserve">saveTask.php med alla parametrar </t>
+  </si>
+  <si>
+    <t>Fel (400) Angiven aktivitet saknas</t>
+  </si>
+  <si>
+    <t>OK Posten sparades</t>
+  </si>
+  <si>
+    <t>Uppdatera uppgift</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar time=-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saveTask.php?id=500 med alla parametrar </t>
+  </si>
+  <si>
+    <t>Fel (400) Angivet id saknas</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar description=''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saveTask.php?id=5 med alla parametrar </t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar activityid=300</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar activityid=tre</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar activityid=-1</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar date=2001-02-29</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar date=tre</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar date=-1</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar time=12:00</t>
+  </si>
+  <si>
+    <t>saveTask.php?id=5 med alla parametrar time=tre</t>
   </si>
 </sst>
 </file>
@@ -760,11 +808,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C2BE4A-9F0B-44D4-B350-F96D596D6606}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1556,6 +1604,15 @@
       <c r="C41" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="D41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1567,8 +1624,17 @@
       <c r="C42" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -1578,8 +1644,17 @@
       <c r="C43" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -1589,8 +1664,17 @@
       <c r="C44" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
@@ -1600,8 +1684,17 @@
       <c r="C45" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>84</v>
       </c>
@@ -1611,8 +1704,17 @@
       <c r="C46" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D46" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>84</v>
       </c>
@@ -1622,8 +1724,17 @@
       <c r="C47" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D47" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>84</v>
       </c>
@@ -1633,8 +1744,17 @@
       <c r="C48" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
@@ -1644,8 +1764,17 @@
       <c r="C49" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
@@ -1655,8 +1784,17 @@
       <c r="C50" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D50" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>84</v>
       </c>
@@ -1666,8 +1804,17 @@
       <c r="C51" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" s="7">
+        <v>44595</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>84</v>
       </c>
@@ -1677,8 +1824,17 @@
       <c r="C52" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E52" s="7">
+        <v>44595</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>84</v>
       </c>
@@ -1688,6 +1844,159 @@
       <c r="C53" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="D53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E53" s="7">
+        <v>44595</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>